<commit_message>
Add continue button handling after successful registration and enhance logging
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -37,7 +37,7 @@
     <t>Pérez</t>
   </si>
   <si>
-    <t>juan.perez+20251109_003734@test.com</t>
+    <t>juan.perez+20251109_004215@test.com</t>
   </si>
   <si>
     <t>3001234567</t>
@@ -52,7 +52,7 @@
     <t>González</t>
   </si>
   <si>
-    <t>maria.gonzalez+20251109_003734@test.com</t>
+    <t>maria.gonzalez+20251109_004215@test.com</t>
   </si>
   <si>
     <t>3007654321</t>
@@ -67,7 +67,7 @@
     <t>Rodríguez</t>
   </si>
   <si>
-    <t>carlos.rodriguez+20251109_003734@test.com</t>
+    <t>carlos.rodriguez+20251109_004215@test.com</t>
   </si>
   <si>
     <t>3009876543</t>
@@ -82,7 +82,7 @@
     <t>Martínez</t>
   </si>
   <si>
-    <t>ana.martinez+20251109_003734@test.com</t>
+    <t>ana.martinez+20251109_004215@test.com</t>
   </si>
   <si>
     <t>3005551234</t>
@@ -97,7 +97,7 @@
     <t>García</t>
   </si>
   <si>
-    <t>luis.garcia+20251109_003734@test.com</t>
+    <t>luis.garcia+20251109_004215@test.com</t>
   </si>
   <si>
     <t>3008887777</t>

</xml_diff>

<commit_message>
Enhance logout and login functionality with improved logging and error handling
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -37,7 +37,7 @@
     <t>Pérez</t>
   </si>
   <si>
-    <t>juan.perez+20251109_004215@test.com</t>
+    <t>juan.perez+20251109_005042@test.com</t>
   </si>
   <si>
     <t>3001234567</t>
@@ -52,7 +52,7 @@
     <t>González</t>
   </si>
   <si>
-    <t>maria.gonzalez+20251109_004215@test.com</t>
+    <t>maria.gonzalez+20251109_005042@test.com</t>
   </si>
   <si>
     <t>3007654321</t>
@@ -67,7 +67,7 @@
     <t>Rodríguez</t>
   </si>
   <si>
-    <t>carlos.rodriguez+20251109_004215@test.com</t>
+    <t>carlos.rodriguez+20251109_005042@test.com</t>
   </si>
   <si>
     <t>3009876543</t>
@@ -82,7 +82,7 @@
     <t>Martínez</t>
   </si>
   <si>
-    <t>ana.martinez+20251109_004215@test.com</t>
+    <t>ana.martinez+20251109_005042@test.com</t>
   </si>
   <si>
     <t>3005551234</t>
@@ -97,7 +97,7 @@
     <t>García</t>
   </si>
   <si>
-    <t>luis.garcia+20251109_004215@test.com</t>
+    <t>luis.garcia+20251109_005042@test.com</t>
   </si>
   <si>
     <t>3008887777</t>

</xml_diff>

<commit_message>
Ajuste de login page
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -37,7 +37,7 @@
     <t>Pérez</t>
   </si>
   <si>
-    <t>juan.perez+20251109_005042@test.com</t>
+    <t>juan.perez+20251109_011412@test.com</t>
   </si>
   <si>
     <t>3001234567</t>
@@ -52,7 +52,7 @@
     <t>González</t>
   </si>
   <si>
-    <t>maria.gonzalez+20251109_005042@test.com</t>
+    <t>maria.gonzalez+20251109_011412@test.com</t>
   </si>
   <si>
     <t>3007654321</t>
@@ -67,7 +67,7 @@
     <t>Rodríguez</t>
   </si>
   <si>
-    <t>carlos.rodriguez+20251109_005042@test.com</t>
+    <t>carlos.rodriguez+20251109_011412@test.com</t>
   </si>
   <si>
     <t>3009876543</t>
@@ -82,7 +82,7 @@
     <t>Martínez</t>
   </si>
   <si>
-    <t>ana.martinez+20251109_005042@test.com</t>
+    <t>ana.martinez+20251109_011412@test.com</t>
   </si>
   <si>
     <t>3005551234</t>
@@ -97,7 +97,7 @@
     <t>García</t>
   </si>
   <si>
-    <t>luis.garcia+20251109_005042@test.com</t>
+    <t>luis.garcia+20251109_011412@test.com</t>
   </si>
   <si>
     <t>3008887777</t>

</xml_diff>

<commit_message>
Refactor login verification to check for "Logout" link instead of "My Account" and enhance error logging in registration process
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -37,7 +37,7 @@
     <t>Pérez</t>
   </si>
   <si>
-    <t>juan.perez+20251109_011412@test.com</t>
+    <t>juan.perez+20251109_012452@test.com</t>
   </si>
   <si>
     <t>3001234567</t>
@@ -52,7 +52,7 @@
     <t>González</t>
   </si>
   <si>
-    <t>maria.gonzalez+20251109_011412@test.com</t>
+    <t>maria.gonzalez+20251109_012452@test.com</t>
   </si>
   <si>
     <t>3007654321</t>
@@ -67,7 +67,7 @@
     <t>Rodríguez</t>
   </si>
   <si>
-    <t>carlos.rodriguez+20251109_011412@test.com</t>
+    <t>carlos.rodriguez+20251109_012452@test.com</t>
   </si>
   <si>
     <t>3009876543</t>
@@ -82,7 +82,7 @@
     <t>Martínez</t>
   </si>
   <si>
-    <t>ana.martinez+20251109_011412@test.com</t>
+    <t>ana.martinez+20251109_012452@test.com</t>
   </si>
   <si>
     <t>3005551234</t>
@@ -97,7 +97,7 @@
     <t>García</t>
   </si>
   <si>
-    <t>luis.garcia+20251109_011412@test.com</t>
+    <t>luis.garcia+20251109_012452@test.com</t>
   </si>
   <si>
     <t>3008887777</t>

</xml_diff>

<commit_message>
Subida a java 21
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -37,7 +37,7 @@
     <t>Pérez</t>
   </si>
   <si>
-    <t>juan.perez+20251109_012452@test.com</t>
+    <t>juan.perez+20251109_013943@test.com</t>
   </si>
   <si>
     <t>3001234567</t>
@@ -52,7 +52,7 @@
     <t>González</t>
   </si>
   <si>
-    <t>maria.gonzalez+20251109_012452@test.com</t>
+    <t>maria.gonzalez+20251109_013943@test.com</t>
   </si>
   <si>
     <t>3007654321</t>
@@ -67,7 +67,7 @@
     <t>Rodríguez</t>
   </si>
   <si>
-    <t>carlos.rodriguez+20251109_012452@test.com</t>
+    <t>carlos.rodriguez+20251109_013943@test.com</t>
   </si>
   <si>
     <t>3009876543</t>
@@ -82,7 +82,7 @@
     <t>Martínez</t>
   </si>
   <si>
-    <t>ana.martinez+20251109_012452@test.com</t>
+    <t>ana.martinez+20251109_013943@test.com</t>
   </si>
   <si>
     <t>3005551234</t>
@@ -97,7 +97,7 @@
     <t>García</t>
   </si>
   <si>
-    <t>luis.garcia+20251109_012452@test.com</t>
+    <t>luis.garcia+20251109_013943@test.com</t>
   </si>
   <si>
     <t>3008887777</t>

</xml_diff>

<commit_message>
Add dump and dumpstream files for test runs with error logs
- Created dump files for test runs on 2025-11-09, capturing thread states and exceptions.
- Included detailed stack traces for EOFExceptions and shutdown commands from Maven.
- Documented thread states and actions for better debugging and analysis of test failures.
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -37,7 +37,7 @@
     <t>Pérez</t>
   </si>
   <si>
-    <t>juan.perez+20251109_013943@test.com</t>
+    <t>juan.perez+20251109_020650@test.com</t>
   </si>
   <si>
     <t>3001234567</t>
@@ -52,7 +52,7 @@
     <t>González</t>
   </si>
   <si>
-    <t>maria.gonzalez+20251109_013943@test.com</t>
+    <t>maria.gonzalez+20251109_020650@test.com</t>
   </si>
   <si>
     <t>3007654321</t>
@@ -67,7 +67,7 @@
     <t>Rodríguez</t>
   </si>
   <si>
-    <t>carlos.rodriguez+20251109_013943@test.com</t>
+    <t>carlos.rodriguez+20251109_020650@test.com</t>
   </si>
   <si>
     <t>3009876543</t>
@@ -82,7 +82,7 @@
     <t>Martínez</t>
   </si>
   <si>
-    <t>ana.martinez+20251109_013943@test.com</t>
+    <t>ana.martinez+20251109_020650@test.com</t>
   </si>
   <si>
     <t>3005551234</t>
@@ -97,7 +97,7 @@
     <t>García</t>
   </si>
   <si>
-    <t>luis.garcia+20251109_013943@test.com</t>
+    <t>luis.garcia+20251109_020650@test.com</t>
   </si>
   <si>
     <t>3008887777</t>

</xml_diff>

<commit_message>
Remove outdated dumpstream files and add test execution report for OpenCart user registration tests, noting failures for all test cases.
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -37,7 +37,7 @@
     <t>Pérez</t>
   </si>
   <si>
-    <t>juan.perez+20251109_020650@test.com</t>
+    <t>juan.perez+20251109_022039@test.com</t>
   </si>
   <si>
     <t>3001234567</t>
@@ -52,7 +52,7 @@
     <t>González</t>
   </si>
   <si>
-    <t>maria.gonzalez+20251109_020650@test.com</t>
+    <t>maria.gonzalez+20251109_022039@test.com</t>
   </si>
   <si>
     <t>3007654321</t>
@@ -67,7 +67,7 @@
     <t>Rodríguez</t>
   </si>
   <si>
-    <t>carlos.rodriguez+20251109_020650@test.com</t>
+    <t>carlos.rodriguez+20251109_022039@test.com</t>
   </si>
   <si>
     <t>3009876543</t>
@@ -82,7 +82,7 @@
     <t>Martínez</t>
   </si>
   <si>
-    <t>ana.martinez+20251109_020650@test.com</t>
+    <t>ana.martinez+20251109_022039@test.com</t>
   </si>
   <si>
     <t>3005551234</t>
@@ -97,7 +97,7 @@
     <t>García</t>
   </si>
   <si>
-    <t>luis.garcia+20251109_020650@test.com</t>
+    <t>luis.garcia+20251109_022039@test.com</t>
   </si>
   <si>
     <t>3008887777</t>

</xml_diff>

<commit_message>
Add dumpstream file for test run on 2025-11-10 with EOFException details
- Created a new dumpstream file to capture the output of the test run.
- Documented the EOFException encountered during the test execution.
- Included stack trace for better debugging and analysis of the issue.
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
   <si>
     <t>First Name</t>
   </si>
@@ -37,7 +37,7 @@
     <t>Pérez</t>
   </si>
   <si>
-    <t>juan.perez+20251110_120951@test.com</t>
+    <t>juan.perez+20251110_130229@test.com</t>
   </si>
   <si>
     <t>3001234567</t>
@@ -52,7 +52,7 @@
     <t>González</t>
   </si>
   <si>
-    <t>maria.gonzalez+20251110_120951@test.com</t>
+    <t>maria.gonzalez+20251110_130229@test.com</t>
   </si>
   <si>
     <t>3007654321</t>
@@ -67,7 +67,7 @@
     <t>Rodríguez</t>
   </si>
   <si>
-    <t>carlos.rodriguez+20251110_120951@test.com</t>
+    <t>carlos.rodriguez+20251110_130229@test.com</t>
   </si>
   <si>
     <t>3009876543</t>
@@ -82,7 +82,7 @@
     <t>Martínez</t>
   </si>
   <si>
-    <t>ana.martinez+20251110_120951@test.com</t>
+    <t>ana.martinez+20251110_130229@test.com</t>
   </si>
   <si>
     <t>3005551234</t>
@@ -97,7 +97,7 @@
     <t>García</t>
   </si>
   <si>
-    <t>luis.garcia+20251110_120951@test.com</t>
+    <t>luis.garcia+20251110_130229@test.com</t>
   </si>
   <si>
     <t>3008887777</t>
@@ -145,43 +145,37 @@
     <t>Cantidad</t>
   </si>
   <si>
-    <t>Desktops</t>
-  </si>
-  <si>
-    <t>PC</t>
-  </si>
-  <si>
-    <t>HP LP3065</t>
+    <t>Laptops &amp; Notebooks</t>
+  </si>
+  <si>
+    <t>MacBook</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>Laptops &amp; Notebooks</t>
-  </si>
-  <si>
-    <t>MacBook</t>
+    <t>iPhone</t>
+  </si>
+  <si>
+    <t>Cameras</t>
+  </si>
+  <si>
+    <t>Canon EOS 5D</t>
+  </si>
+  <si>
+    <t>Macs</t>
+  </si>
+  <si>
+    <t>MacBook Air</t>
   </si>
   <si>
     <t>2</t>
   </si>
   <si>
-    <t>Components</t>
-  </si>
-  <si>
-    <t>Monitors</t>
-  </si>
-  <si>
-    <t>Apple Cinema 30</t>
-  </si>
-  <si>
-    <t>iPhone</t>
-  </si>
-  <si>
-    <t>Cameras</t>
-  </si>
-  <si>
-    <t>Canon EOS 5D</t>
+    <t>Tablets</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy Tab 10.1</t>
   </si>
 </sst>
 </file>
@@ -486,7 +480,7 @@
   <cols>
     <col min="1" max="1" width="18.23046875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="11.84765625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="14.515625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="21.24609375" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="8.28515625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -509,69 +503,69 @@
         <v>43</v>
       </c>
       <c r="B2" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s" s="0">
         <v>44</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="D2" t="s" s="0">
         <v>45</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>46</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s" s="0">
         <v>36</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s" s="0">
         <v>36</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove obsolete dumpstream file and update test class binaries; add detailed test execution logs for user registration and login tests.
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -37,7 +37,7 @@
     <t>Pérez</t>
   </si>
   <si>
-    <t>juan.perez+20251110_130229@test.com</t>
+    <t>juan.perez+20251111_202811@test.com</t>
   </si>
   <si>
     <t>3001234567</t>
@@ -52,7 +52,7 @@
     <t>González</t>
   </si>
   <si>
-    <t>maria.gonzalez+20251110_130229@test.com</t>
+    <t>maria.gonzalez+20251111_202811@test.com</t>
   </si>
   <si>
     <t>3007654321</t>
@@ -67,7 +67,7 @@
     <t>Rodríguez</t>
   </si>
   <si>
-    <t>carlos.rodriguez+20251110_130229@test.com</t>
+    <t>carlos.rodriguez+20251111_202811@test.com</t>
   </si>
   <si>
     <t>3009876543</t>
@@ -82,7 +82,7 @@
     <t>Martínez</t>
   </si>
   <si>
-    <t>ana.martinez+20251110_130229@test.com</t>
+    <t>ana.martinez+20251111_202811@test.com</t>
   </si>
   <si>
     <t>3005551234</t>
@@ -97,7 +97,7 @@
     <t>García</t>
   </si>
   <si>
-    <t>luis.garcia+20251110_130229@test.com</t>
+    <t>luis.garcia+20251111_202811@test.com</t>
   </si>
   <si>
     <t>3008887777</t>

</xml_diff>

<commit_message>
Ajustes y subida de documentacion final
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -37,7 +37,7 @@
     <t>Pérez</t>
   </si>
   <si>
-    <t>juan.perez+20251111_202811@test.com</t>
+    <t>juan.perez+20251112_211458@test.com</t>
   </si>
   <si>
     <t>3001234567</t>
@@ -52,7 +52,7 @@
     <t>González</t>
   </si>
   <si>
-    <t>maria.gonzalez+20251111_202811@test.com</t>
+    <t>maria.gonzalez+20251112_211458@test.com</t>
   </si>
   <si>
     <t>3007654321</t>
@@ -67,7 +67,7 @@
     <t>Rodríguez</t>
   </si>
   <si>
-    <t>carlos.rodriguez+20251111_202811@test.com</t>
+    <t>carlos.rodriguez+20251112_211458@test.com</t>
   </si>
   <si>
     <t>3009876543</t>
@@ -82,7 +82,7 @@
     <t>Martínez</t>
   </si>
   <si>
-    <t>ana.martinez+20251111_202811@test.com</t>
+    <t>ana.martinez+20251112_211458@test.com</t>
   </si>
   <si>
     <t>3005551234</t>
@@ -97,7 +97,7 @@
     <t>García</t>
   </si>
   <si>
-    <t>luis.garcia+20251111_202811@test.com</t>
+    <t>luis.garcia+20251112_211458@test.com</t>
   </si>
   <si>
     <t>3008887777</t>

</xml_diff>

<commit_message>
Add end-to-end purchase test and update test suite
- Introduced `ComprarTest` class for end-to-end purchase testing.
- Updated `testng.xml` to include the new purchase test.
- Generated execution logs for the purchase test, detailing user actions and outcomes.
- Created Surefire reports for the new test, confirming successful execution with no failures or errors.
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -37,7 +37,7 @@
     <t>Pérez</t>
   </si>
   <si>
-    <t>juan.perez+20251112_211458@test.com</t>
+    <t>juan.perez+20251112_215226@test.com</t>
   </si>
   <si>
     <t>3001234567</t>
@@ -52,7 +52,7 @@
     <t>González</t>
   </si>
   <si>
-    <t>maria.gonzalez+20251112_211458@test.com</t>
+    <t>maria.gonzalez+20251112_215226@test.com</t>
   </si>
   <si>
     <t>3007654321</t>
@@ -67,7 +67,7 @@
     <t>Rodríguez</t>
   </si>
   <si>
-    <t>carlos.rodriguez+20251112_211458@test.com</t>
+    <t>carlos.rodriguez+20251112_215226@test.com</t>
   </si>
   <si>
     <t>3009876543</t>
@@ -82,7 +82,7 @@
     <t>Martínez</t>
   </si>
   <si>
-    <t>ana.martinez+20251112_211458@test.com</t>
+    <t>ana.martinez+20251112_215226@test.com</t>
   </si>
   <si>
     <t>3005551234</t>
@@ -97,7 +97,7 @@
     <t>García</t>
   </si>
   <si>
-    <t>luis.garcia+20251112_211458@test.com</t>
+    <t>luis.garcia+20251112_215226@test.com</t>
   </si>
   <si>
     <t>3008887777</t>

</xml_diff>